<commit_message>
Minor Changes to Planning Documents
Made some minor updates to planning documents, notably time spent in the time log.
</commit_message>
<xml_diff>
--- a/planning/TimeLog.xlsx
+++ b/planning/TimeLog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Yeti Mountain Time Log</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>BearLibTerminal .ini edits</t>
+  </si>
+  <si>
+    <t>Setting up Basic ECS project in GitHub</t>
   </si>
 </sst>
 </file>
@@ -421,11 +424,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +514,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:D2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ECS Progress - Entity, Position and Character
#1 has been completed for now; new components will be added to it as we
go. #2 is in progress; I need to add direction to the position component
and will probably change 'character' to 'glyph.
</commit_message>
<xml_diff>
--- a/planning/TimeLog.xlsx
+++ b/planning/TimeLog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RL\YetiMountain\YetiMountain\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daeri\Documents\RLs\YetiMountain\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Yeti Mountain Time Log</t>
   </si>
@@ -60,12 +60,15 @@
   </si>
   <si>
     <t>Setting up Basic ECS project in GitHub</t>
+  </si>
+  <si>
+    <t>Programming basic ECS during Data Communications Class</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,28 +426,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -458,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43124</v>
       </c>
@@ -472,7 +475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43125</v>
       </c>
@@ -486,7 +489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43126</v>
       </c>
@@ -500,7 +503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43126</v>
       </c>
@@ -514,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43129</v>
       </c>
@@ -528,8 +531,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:D2"/>
+  <autoFilter ref="A2:D2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Log for finishing BasicECS
added a row to the log
</commit_message>
<xml_diff>
--- a/planning/TimeLog.xlsx
+++ b/planning/TimeLog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Yeti Mountain Time Log</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Programming</t>
+  </si>
+  <si>
+    <t>Added RenderingSystem and completed Basic ECS</t>
   </si>
 </sst>
 </file>
@@ -439,11 +442,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,6 +599,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:E2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>